<commit_message>
The page_finder code can now scrape multiple pages. Saving name, url, price and ave rating. Next step is to merge it with the review_scraper.
</commit_message>
<xml_diff>
--- a/product_urls.xlsx
+++ b/product_urls.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
-  <si>
-    <t>name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="140">
+  <si>
+    <t>description</t>
   </si>
   <si>
     <t>url</t>
@@ -28,196 +28,412 @@
     <t>rating</t>
   </si>
   <si>
-    <t>num_of_ratings</t>
-  </si>
-  <si>
-    <t>LEGO Everyone is Awesome Set 40516</t>
-  </si>
-  <si>
-    <t>LEGO Marvel Super Heroes S.H.I.E.L.D. - Maria Hill (76042)</t>
-  </si>
-  <si>
-    <t>LEGO Parts - Crocodile/Aligator. Dark green with yellow eyes. by LEGO</t>
-  </si>
-  <si>
-    <t>LEGO 76239 DC Batman Batmobile Tumbler: Scarecrow Showdown Toy Car with Batman and Scarecrow Minifigures, for Kids Age 8</t>
+    <t>page</t>
+  </si>
+  <si>
+    <t>LEGO 40220 Blocks</t>
+  </si>
+  <si>
+    <t>Lego Prince of Persia Mini Figure - Skeleton</t>
+  </si>
+  <si>
+    <t>LEGO Jurassic World (75936) Confidential, Bunt</t>
+  </si>
+  <si>
+    <t>LEGO 75301 Star Wars Luke Skywalker's X-Wing Fighter Toy for Kids Age 9+ with Princess Leia Minifigure and R2-D2 Droid Figure</t>
+  </si>
+  <si>
+    <t>LEGO 42110 Technic Land Rover Defender Off Road 4x4 Car, Exclusive Collectible Model, Advanced Building Set</t>
+  </si>
+  <si>
+    <t>LEGO 10281 Creator Expert Bonsai Tree Set for Adults, Home Décor DIY Projects, Botanical Collection</t>
   </si>
   <si>
     <t>LEGO 42123 Technic McLaren Senna GTR Racing Sports Car Collectible Model, Vehicle Construction Set</t>
   </si>
   <si>
-    <t>LEGO 10281 Creator Expert Bonsai Tree Set for Adults, Home Décor DIY Projects, Botanical Collection</t>
-  </si>
-  <si>
-    <t>LEGO 41445 Friends Vet Clinic Ambulance Toy Car, Animal Rescue Playset with Olivia and Emma Minidolls</t>
-  </si>
-  <si>
-    <t>LEGO 42110 Technic Land Rover Defender Off Road 4x4 Car, Exclusive Collectible Model, Advanced Building Set</t>
+    <t>LEGO 75957 Harry Potter - The Knight Bus (Triple-decker Set with Minifigures)</t>
+  </si>
+  <si>
+    <t>LEGO 60281 City Fire Rescue Helicopter Toy with Motorbike, Firefighter and Pilot Minifigures</t>
+  </si>
+  <si>
+    <t>LEGO 41679 Friends Forest House Toy, Treehouse Adventure Set with Mia Mini Doll and Kayak Boat Model</t>
+  </si>
+  <si>
+    <t>LEGO 76191 Marvel Infinity Gauntlet Building Set, Thanos Glove Model for Adults, Collectible Avengers Gift</t>
+  </si>
+  <si>
+    <t>LEGO 76169 Super Heroes Marvel Avengers Thor Mech Armour Set, Action Figure Toy with Thor Minifigure</t>
+  </si>
+  <si>
+    <t>LEGO 41441 Friends Horse Training and Trailer Building Set with Stables and Car, Toy for Kids 4+ Years Old</t>
+  </si>
+  <si>
+    <t>LEGO 75318 Star Wars: The Mandalorian The Child Baby Yoda Figure Gift Idea</t>
   </si>
   <si>
     <t>LEGO 60303 City Advent Calendar 2021 Mini Builds Set, Christmas Toys for Kids Age 5 with Play Board &amp; 6 Minifigures</t>
   </si>
   <si>
+    <t>LEGO 31088 Creator Deep Sea Creatures: Shark, Crab and Squid or Angler Fish, 3 in 1 Seaside Adventures Building Set, Toys for Kids 7 Years Old and Older</t>
+  </si>
+  <si>
+    <t>LEGO 60276 City Police Prisoner Transport Tow Truck Toy, Police Station Expansion Set</t>
+  </si>
+  <si>
+    <t>LEGO 60283 City Great Vehicles Holiday Camper Van Toy, Motorhome Car Playset, Summer Holidays Toys</t>
+  </si>
+  <si>
     <t>LEGO 42121 Technic Heavy-Duty Excavator Toy, 2 in 1 Model, Construction Vehicle Building Set for Kids 8 Years Old</t>
   </si>
   <si>
-    <t>LEGO 60281 City Fire Rescue Helicopter Toy with Motorbike, Firefighter and Pilot Minifigures</t>
-  </si>
-  <si>
-    <t>LEGO 60283 City Great Vehicles Holiday Camper Van Toy, Motorhome Car Playset, Summer Holidays Toys</t>
-  </si>
-  <si>
-    <t>LEGO 76169 Super Heroes Marvel Avengers Thor Mech Armour Set, Action Figure Toy with Thor Minifigure</t>
-  </si>
-  <si>
-    <t>LEGO 76195 Marvel Spider-Man’s Drone Duel Building Toy for Kids Age 7 , Superhero Birthday Idea</t>
+    <t>LEGO 42119 Technic Monster Jam Max-D Truck Toy to Quad Bike Pull Back 2 in 1 Building Set</t>
+  </si>
+  <si>
+    <t>LEGO 75312 Star Wars Boba Fett’s Starship Building Toy for Kids Age 9 , Mandalorian Model Set with 2 Minifigures</t>
+  </si>
+  <si>
+    <t>LEGO 75314 Star Wars The Bad Batch Attack Shuttle Building Toy for Kids Age 9 , Set with 5 Clones Minifigures &amp; Gonk Droid Figure</t>
   </si>
   <si>
     <t>LEGO 21159 Minecraft The Pillager Outpost Action Figures Building Set, Iron Golem Adventure Toy for Kids 7 Years Old</t>
   </si>
   <si>
-    <t>LEGO 75314 Star Wars The Bad Batch Attack Shuttle Building Toy for Kids Age 9 , Set with 5 Clones Minifigures &amp; Gonk Droid Figure</t>
-  </si>
-  <si>
-    <t>LEGO 75301 Star Wars Luke Skywalker's X-Wing Fighter Toy for Kids Age 9+ with Princess Leia Minifigure and R2-D2 Droid Figure</t>
-  </si>
-  <si>
-    <t>LEGO 75312 Star Wars Boba Fett’s Starship Building Toy for Kids Age 9 , Mandalorian Model Set with 2 Minifigures</t>
-  </si>
-  <si>
-    <t>LEGO 75311 Star Wars Imperial Armoured Marauder Building Toy for Kids Age 8 , Mandalorian Model Set with 4 Minifigures</t>
-  </si>
-  <si>
-    <t>LEGO 75957 Harry Potter - The Knight Bus (Triple-decker Set with Minifigures)</t>
-  </si>
-  <si>
-    <t>LEGO 76940 Jurassic World T. rex Dinosaur Fossil Exhibition Toy Playset for Kids Age 7+, Skeleton Model Building Set</t>
+    <t>LEGO 60288 City Great Vehicles Race Buggy Transporter  Toy Truck with Trailer and Steerable Baja Race Car</t>
+  </si>
+  <si>
+    <t>LEGO 42122 Technic Jeep Wrangler 4x4 Toy Car, Off Roader SUV Model Building Set</t>
   </si>
   <si>
     <t>LEGO 21166 Minecraft The Abandoned Mine Building Set, Zombie Cave with Slime, Steve and Spider Figures</t>
   </si>
   <si>
+    <t>LEGO 76387 Harry Potter Hogwarts: Fluffy Encounter Castle Toy Building Set, with 20th Anniversary Golden Minifigure &amp; 3-Headed Dog Figure</t>
+  </si>
+  <si>
     <t>LEGO 21034 Architecture Skyline Model Building Set, London Eye, Big Ben, Tower Bridge Collection, Construction Collectible Gift Idea</t>
   </si>
   <si>
-    <t>LEGO 60288 City Great Vehicles Race Buggy Transporter  Toy Truck with Trailer and Steerable Baja Race Car</t>
-  </si>
-  <si>
-    <t>LEGO 60276 City Police Prisoner Transport Tow Truck Toy, Police Station Expansion Set</t>
+    <t>LEGO 10692 Classic Creative Bricks, Classic Colorful Building Set with Storage Box (221 Pieces)</t>
+  </si>
+  <si>
+    <t>LEGO 76196 Marvel The Avengers Advent Calendar 2021 Buildable Toys with Spider-Man and Iron Man for Kids Aged 7 Idea</t>
+  </si>
+  <si>
+    <t>LEGO 75307 Star Wars Advent Calendar 2021 Toy Building Set, The Mandalorian for Kids Age 6 with Baby Yoda Minifigure</t>
   </si>
   <si>
     <t>LEGO 76186 Marvel Black Panther Dragon Flyer, Avengers Building Toy with 3 Minifigures, Super Heroes Set</t>
   </si>
   <si>
-    <t>LEGO 31088 Creator Deep Sea Creatures: Shark, Crab and Squid or Angler Fish, 3 in 1 Seaside Adventures Building Set, Toys for Kids 7 Years Old and Older</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_toys_sr_pg1_1?ie=UTF8&amp;adId=A04895281IWVRTD8UPZM2&amp;url=%2FLEGO-Everyone-Awesome-Set-40516%2Fdp%2FB09698FGPL%2Fref%3Dsr_1_1_sspa%3Fcrid%3D1SDTYPYXM70YV%26dchild%3D1%26keywords%3Dlego%26qid%3D1634474215%26refinements%3Dp_89%253Alego%26rnid%3D1632651031%26s%3Dkids%26sprefix%3Dmy%2Bli%252Ctoys%252C163%26sr%3D1-1-spons%26psc%3D1%26smid%3DA1QD8OYV8FUXRI&amp;qualifier=1634474215&amp;id=4928294116655482&amp;widgetName=sp_atf</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_toys_sr_pg1_1?ie=UTF8&amp;adId=A01423763NPOLBBDWQ5ZI&amp;url=%2FLEGO-Marvel-Super-Heroes-S-H-I%2Fdp%2FB0100ZTRPI%2Fref%3Dsr_1_2_sspa%3Fcrid%3D1SDTYPYXM70YV%26dchild%3D1%26keywords%3Dlego%26qid%3D1634474215%26refinements%3Dp_89%253Alego%26rnid%3D1632651031%26s%3Dkids%26sprefix%3Dmy%2Bli%252Ctoys%252C163%26sr%3D1-2-spons%26psc%3D1&amp;qualifier=1634474215&amp;id=4928294116655482&amp;widgetName=sp_atf</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_toys_sr_pg1_1?ie=UTF8&amp;adId=A0225253Q9GWSJDGFCHV&amp;url=%2FLEGO-Parts-Crocodile-Aligator-yellow%2Fdp%2FB013S76TL0%2Fref%3Dsr_1_3_sspa%3Fcrid%3D1SDTYPYXM70YV%26dchild%3D1%26keywords%3Dlego%26qid%3D1634474215%26refinements%3Dp_89%253Alego%26rnid%3D1632651031%26s%3Dkids%26sprefix%3Dmy%2Bli%252Ctoys%252C163%26sr%3D1-3-spons%26psc%3D1%26smid%3DA1HZWI0Z8OAQOE&amp;qualifier=1634474215&amp;id=4928294116655482&amp;widgetName=sp_atf</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-76239-Batman-Batmobile-Tumbler/dp/B08WX6R3KY/ref=sr_1_4?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-4</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-42123-Technic-Collectible-Construction/dp/B08G4293BD/ref=sr_1_5?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-5</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-10281-LEGO-10281-Creator-Expert-Bonsai-Tree-Set-for-Adults-Home-D%C3%A9cor-DIY-Projects-Botanical-Collection/dp/B08G4PCG8F/ref=sr_1_6?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-6</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-41445-Friends-Ambulance-Minidolls/dp/B08G4DRGBQ/ref=sr_1_7?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-7</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-42110-Toy-Multicolour/dp/B07P2GQDQ6/ref=sr_1_8?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-8</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-60303-Calendar-Christmas-Minifigures/dp/B08X1B622Z/ref=sr_1_9?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-9</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-42121-Heavy-Duty-Excavator-Construction/dp/B08G4CKL16/ref=sr_1_10?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-10</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-60281-Helicopter-Firefighter-Minifigures/dp/B08G4D3P1T/ref=sr_1_11?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-11</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-60283-Vehicles-Motorhome-Holidays/dp/B08G4M8J87/ref=sr_1_12?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-12</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-76169-Heroes-Avengers-Minifigure/dp/B08G4B5Z97/ref=sr_1_13?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-13</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-76195-tbd-LSH-2021/dp/B08W9HBYV7/ref=sr_1_14?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-14</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-21159-LEGO-21159-Minecraft-The-Pillager-Outpost-Action-Figures-Building-Set-Iron-Golem-Adventure-Toy-for-Kids-7-Years-Old/dp/B07WC1VFZH/ref=sr_1_15?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-15</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-75314-Shuttle-Building-Minifigures/dp/B08WWKYKT9/ref=sr_1_16?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-16</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-75301-Skywalkers-Fighter-Princess/dp/B08G4GP34B/ref=sr_1_17?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-17</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-75312-Starship-Mandalorian-Minifigures/dp/B08WWTPDG2/ref=sr_1_18?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-18</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-75311-Imperial-Mandalorian-Minifigures/dp/B08WB22HQY/ref=sr_1_19?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-19</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-75957-Triple-decker-Collectible-Minifigures/dp/B07KX54VHF/ref=sr_1_20?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-20</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-tbd-dino-1-2021/dp/B08W9TBGLJ/ref=sr_1_21?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-21</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-21166-Minecraft-Abandoned-Building/dp/B085WV4WST/ref=sr_1_22?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-22</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-21034-Architecture-Skyline-Building/dp/B01J41MPF8/ref=sr_1_23?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-23</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-60288-Vehicles-Transporter-Steerable/dp/B08G4LMHB4/ref=sr_1_24?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-24</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-60276-Prisoner-Transport-Expansion/dp/B08G4PBFLQ/ref=sr_1_25?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-25</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-76186-Avengers-Building-Minifigures/dp/B08W8KPVKC/ref=sr_1_26?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-26</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/LEGO-31088-Creatures-Building-Colourful/dp/B07FNS6J7R/ref=sr_1_27?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634474215&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-27</t>
+    <t>LEGO 42111 Technic Fast &amp; Furious Dom's Dodge Charger Racing Car Model Iconic Collector's Building Set</t>
+  </si>
+  <si>
+    <t>LEGO 76190 Marvel Iron Man Monger Mayhem Set, Avengers Mech Building Toy, Action Figure for Kids 9+ Years Old</t>
+  </si>
+  <si>
+    <t>LEGO 42096 Technic  Porsche 911 RSR Race Car Advanced Building Set, Exclusive Collectible Model</t>
+  </si>
+  <si>
+    <t>LEGO 21028 Architecture New York City Skyline Building Set</t>
+  </si>
+  <si>
+    <t>LEGO 76388 Harry Potter Hogsmeade Village Visit 20th Anniversary Set with Collectible Golden Minifigure</t>
+  </si>
+  <si>
+    <t>LEGO 75306 Star Wars Imperial Probe Droid Building Set for Adults, Collectible Gift for The Empire Strikes Back Fans</t>
+  </si>
+  <si>
+    <t>LEGO 60287 City Great Vehicles Tractor Toy, Farm Set with Rabbit Figure for 5 Years Old Boys and Girls</t>
+  </si>
+  <si>
+    <t>LEGO 60139 City Police Mobile Command Center Building Set, truck toy and Motorbike, Police Toys for Kids</t>
+  </si>
+  <si>
+    <t>LEGO 75979 Harry Potter Hedwig the Owl Figure Collectible Display Model with Moving Wings</t>
+  </si>
+  <si>
+    <t>LEGO 60298 City Stuntz Rocket Stunt Bike Set with Flywheel-Powered Toy Motorbike &amp; Rocket Racer Minifigure, Toys for Kids 5 Years Old</t>
+  </si>
+  <si>
+    <t>LEGO 76900 Speed Champions Koenigsegg Jesko Racing Sports Car Toy with Driver Minifigure, Racer Model Set for Kids</t>
+  </si>
+  <si>
+    <t>LEGO 41443 Friends Olivia's Electric Car Toy, Eco Education Playset for Kids 6</t>
+  </si>
+  <si>
+    <t>LEGO 31111 Creator 3 in 1 Cyber Drone Building Set with Cyber Mech and Scooter, Space Toys for Kids 6 Years Old</t>
+  </si>
+  <si>
+    <t>LEGO 42120 Technic Rescue Hovercraft to Aircraft Toy, 2 in 1 Model, Building Set for Boys and Girls 8 + Years Old</t>
+  </si>
+  <si>
+    <t>LEGO 60198 City Cargo Train Set Battery Powered Engine For 6 Year Old, RC Bluetooth Connection, 3 Wagons, Tracks and Accessories</t>
+  </si>
+  <si>
+    <t>LEGO 76902 Speed Champions McLaren Elva Racing Car Toy for Kids 7+ Years Old, Sports Race Model Building Set</t>
+  </si>
+  <si>
+    <t>LEGO 60226 City Mars Research Shuttle Spaceship Construction Toys for Kids inspired by NASA with Rover and Drone</t>
+  </si>
+  <si>
+    <t>LEGO 71381 Super Mario Chain Chomp Jungle Encounter Expansion Set, Buildable Game with Bramball Figure</t>
+  </si>
+  <si>
+    <t>LEGO 75298 Star Wars AT-AT vs. Tauntaun Microfighters  Building Set with Luke Skywalker and AT-AT Driver Minifigures</t>
+  </si>
+  <si>
+    <t>LEGO 75300 Star Wars Imperial TIE Fighter Toy with Stormtrooper and Pilot Minifigures from The Skywalker Saga</t>
+  </si>
+  <si>
+    <t>LEGO 92176 Ideas NASA Apollo Saturn V Space Rocket and Vehicles, Spaceship Collectors Building Set with Display Stand [Amazon Exclusive]</t>
+  </si>
+  <si>
+    <t>LEGO 76168 Marvel Avengers Captain America Mech Armour Set, Action Figure Toy for 7+ Years Old Boys and Girls</t>
+  </si>
+  <si>
+    <t>LEGO 71746 NINJAGO Jungle Dragon Building Set, with Ninja Lloyd and Zane Minifigures, Toys for 8 + Years Old Boys and Girls</t>
+  </si>
+  <si>
+    <t>LEGO 41938 DOTS Creative Designer Box, Lots of Extra DOTS, with Pencil Holder, Desk Organiser, Picture Frame &amp; Door Sign for Kids</t>
+  </si>
+  <si>
+    <t>LEGO 71745 NINJAGO Lloyd’s Jungle Chopper Bike Building Set, Motorbike Toy with Lloyd and Nya Minifigures</t>
+  </si>
+  <si>
+    <t>LEGO 21165 Minecraft The Bee Farm Village Building Set with Beekeeper and Sheep Figure, Toys 8 Boys and Girls</t>
+  </si>
+  <si>
+    <t>LEGO 75948 Harry Potter Hogwarts Castle Clock Tower Toy, Compatible with Great Hall and Whomping Willow Sets</t>
+  </si>
+  <si>
+    <t>LEGO 41444 Friends Heartlake City Organic Café Playset, Eco Education for Kids 6+</t>
+  </si>
+  <si>
+    <t>LEGO Elfen-Klubhaus (10275) 1192 Teile</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_toys_sr_pg1_1?ie=UTF8&amp;adId=A05703253Q7UGAOUXA9OZ&amp;url=%2FLEGO-Creator-London-40220-361329%2Fdp%2FB01KSGLLLM%2Fref%3Dsr_1_1_sspa%3Fcrid%3D1SDTYPYXM70YV%26dchild%3D1%26keywords%3Dlego%26qid%3D1634570184%26refinements%3Dp_89%253Alego%26rnid%3D1632651031%26s%3Dkids%26sprefix%3Dmy%2Bli%252Ctoys%252C163%26sr%3D1-1-spons%26psc%3D1%26smid%3DA2672SK7B2U42P&amp;qualifier=1634570184&amp;id=2457982534738217&amp;widgetName=sp_atf</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_toys_sr_pg1_1?ie=UTF8&amp;adId=A01687702O7RFQ4SBKN16&amp;url=%2FLego-Prince-Persia-Mini-Figure%2Fdp%2FB003IUQYCW%2Fref%3Dsr_1_2_sspa%3Fcrid%3D1SDTYPYXM70YV%26dchild%3D1%26keywords%3Dlego%26qid%3D1634570184%26refinements%3Dp_89%253Alego%26rnid%3D1632651031%26s%3Dkids%26sprefix%3Dmy%2Bli%252Ctoys%252C163%26sr%3D1-2-spons%26psc%3D1%26smid%3DA1HZWI0Z8OAQOE&amp;qualifier=1634570184&amp;id=2457982534738217&amp;widgetName=sp_atf</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/gp/slredirect/picassoRedirect.html/ref=pa_sp_atf_toys_sr_pg1_1?ie=UTF8&amp;adId=A04688572CLN0WDINMNI6&amp;url=%2FLEGO-Jurassic-World-75936-Confidential-Multi-Coloured%2Fdp%2FB07G3RKS79%2Fref%3Dsr_1_3_sspa%3Fcrid%3D1SDTYPYXM70YV%26dchild%3D1%26keywords%3Dlego%26qid%3D1634570184%26refinements%3Dp_89%253Alego%26rnid%3D1632651031%26s%3Dkids%26sprefix%3Dmy%2Bli%252Ctoys%252C163%26sr%3D1-3-spons%26psc%3D1%26smid%3DA1QD8OYV8FUXRI&amp;qualifier=1634570184&amp;id=2457982534738217&amp;widgetName=sp_atf</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75301-Skywalkers-Fighter-Princess/dp/B08G4GP34B/ref=sr_1_4?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-4</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42110-Toy-Multicolour/dp/B07P2GQDQ6/ref=sr_1_5?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-5</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-10281-LEGO-10281-Creator-Expert-Bonsai-Tree-Set-for-Adults-Home-D%C3%A9cor-DIY-Projects-Botanical-Collection/dp/B08G4PCG8F/ref=sr_1_6?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-6</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42123-Technic-Collectible-Construction/dp/B08G4293BD/ref=sr_1_7?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-7</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75957-Triple-decker-Collectible-Minifigures/dp/B07KX54VHF/ref=sr_1_8?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-8</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60281-Helicopter-Firefighter-Minifigures/dp/B08G4D3P1T/ref=sr_1_9?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-9</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-41679-Friends-Treehouse-Adventure/dp/B08W5FXSQJ/ref=sr_1_10?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-10</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76191-Infinity-Gauntlet-Collectible/dp/B08WX4YRK7/ref=sr_1_11?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-11</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76169-Heroes-Avengers-Minifigure/dp/B08G4B5Z97/ref=sr_1_12?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-12</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-41441-Friends-Training-Building/dp/B08W5FF49K/ref=sr_1_13?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-13</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75318-Star-Wars-Mandalorian/dp/B085WV2WGC/ref=sr_1_14?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-14</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60303-Calendar-Christmas-Minifigures/dp/B08X1B622Z/ref=sr_1_15?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-15</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-31088-Creatures-Building-Colourful/dp/B07FNS6J7R/ref=sr_1_16?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-16</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60276-Prisoner-Transport-Expansion/dp/B08G4PBFLQ/ref=sr_1_17?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-17</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60283-Vehicles-Motorhome-Holidays/dp/B08G4M8J87/ref=sr_1_18?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-18</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42121-Heavy-Duty-Excavator-Construction/dp/B08G4CKL16/ref=sr_1_19?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-19</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42119-Technic-Monster-Building/dp/B08G4D31L2/ref=sr_1_20?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-20</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75312-Starship-Mandalorian-Minifigures/dp/B08WWTPDG2/ref=sr_1_21?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-21</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75314-Shuttle-Building-Minifigures/dp/B08WWKYKT9/ref=sr_1_22?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-22</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-21159-LEGO-21159-Minecraft-The-Pillager-Outpost-Action-Figures-Building-Set-Iron-Golem-Adventure-Toy-for-Kids-7-Years-Old/dp/B07WC1VFZH/ref=sr_1_23?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-23</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60288-Vehicles-Transporter-Steerable/dp/B08G4LMHB4/ref=sr_1_24?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-24</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42122-Technic-Wrangler-Building/dp/B08G4LZVTW/ref=sr_1_25?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-25</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-21166-Minecraft-Abandoned-Building/dp/B085WV4WST/ref=sr_1_26?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-26</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76387-Harry-Potter-Hogwarts/dp/B08W8LDL1F/ref=sr_1_27?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570184&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-27</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42122-Technic-Wrangler-Building/dp/B08G4LZVTW/ref=sr_1_25?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-25</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75318-Star-Wars-Mandalorian/dp/B085WV2WGC/ref=sr_1_26?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-26</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-31088-Creatures-Building-Colourful/dp/B07FNS6J7R/ref=sr_1_27?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-27</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42119-Technic-Monster-Building/dp/B08G4D31L2/ref=sr_1_28?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-28</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60276-Prisoner-Transport-Expansion/dp/B08G4PBFLQ/ref=sr_1_29?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-29</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-21034-Architecture-Skyline-Building/dp/B01J41MPF8/ref=sr_1_30?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-30</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-10692-Creative-Learning-Children/dp/B00NVDOWUW/ref=sr_1_31?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-31</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76196-tbd-LSH-29-2021/dp/B08W9GQ7MV/ref=sr_1_32?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-32</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75307-tbd-IP-LSW14-2021/dp/B08W9K2CTM/ref=sr_1_33?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-33</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76186-Avengers-Building-Minifigures/dp/B08W8KPVKC/ref=sr_1_34?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-34</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42111-Technic-Collectors-Building/dp/B07YYQ89RT/ref=sr_1_35?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-35</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76190-Marvel-Avengers-Building/dp/B08WX3FDC2/ref=sr_1_36?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-36</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/42096-Technic-Building-Realistic-Construction/dp/B07FP6QNQ7/ref=sr_1_37?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-37</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-21028-Architecture-Skyline-Collection/dp/B012NOGGHQ/ref=sr_1_38?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-38</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76388-Anniversary-Collectible-Minifigure/dp/B08WXFFY9F/ref=sr_1_39?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-39</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75306-Toy/dp/B08G46Q9YD/ref=sr_1_40?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-40</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60287-Vehicles-Tractor-Rabbit/dp/B08G4THL9P/ref=sr_1_41?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-41</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60139-Command-Building-Motorbike/dp/B01J41G4SC/ref=sr_1_42?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-42</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/gp/slredirect/picassoRedirect.html/ref=pa_sp_mtf_toys_sr_pg2_1?ie=UTF8&amp;adId=A05703253Q7UGAOUXA9OZ&amp;url=%2FLEGO-Creator-London-40220-361329%2Fdp%2FB01KSGLLLM%2Fref%3Dsr_1_43_sspa%3Fcrid%3D1SDTYPYXM70YV%26dchild%3D1%26keywords%3Dlego%26qid%3D1634570187%26refinements%3Dp_89%253Alego%26rnid%3D1632651031%26s%3Dkids%26sprefix%3Dmy%2Bli%252Ctoys%252C163%26sr%3D1-43-spons%26psc%3D1%26smid%3DA2672SK7B2U42P&amp;qualifier=1634570187&amp;id=1926288755431808&amp;widgetName=sp_mtf</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/75979-Harry-Potter-Collectible-Display/dp/B0813S3VDM/ref=sr_1_44?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-44</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60298-Rocket-Stunt-Bike/dp/B08W5FWDRT/ref=sr_1_45?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-45</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76900-Champions-Koenigsegg-Minifigure/dp/B08W8W71HC/ref=sr_1_46?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-46</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-41443-Friends-Electric-Education/dp/B08G4BMD2K/ref=sr_1_47?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-47</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-31111-Creator-Building-Scooter/dp/B08G4MH27V/ref=sr_1_48?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-48</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-42120-Hovercraft-Aircraft-Building/dp/B08G4SR6C8/ref=sr_1_49?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570187&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-49</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60198-Cargo-Train-Multicolored/dp/B078K4K423/ref=sr_1_49?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-49</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76902-Champions-McLaren-Building/dp/B08W8H6KCC/ref=sr_1_50?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-50</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-60226-navette-spatiale-Multicolour/dp/B07KTVJHPF/ref=sr_1_51?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-51</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-71381-Encounter-Expansion-Buildable/dp/B08G4FD6BL/ref=sr_1_52?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-52</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75298-Microfighters-Skywalker-Minifigures/dp/B08G4CNSJQ/ref=sr_1_53?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-53</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-75300-Stormtrooper-Minifigures-Skywalker/dp/B08G444BQH/ref=sr_1_54?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-54</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-92176-LEGO-92176-Ideas-NASA-Apollo-Saturn-V-Space-Rocket-and-Vehicles-Spaceship-Collectors-Building-Set-with-Display-Stand/dp/B08GNXNPR6/ref=sr_1_55?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-55</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-76168-Avengers-Captain-America/dp/B08G44WXWR/ref=sr_1_56?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-56</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-71746-NINJAGO-Building-Minifigures/dp/B08G46PN5C/ref=sr_1_57?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-57</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-41938-Creative-Designer-Organiser/dp/B08WWTMGCQ/ref=sr_1_58?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-58</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-71745-Building-Motorbike-Minifigures/dp/B08G4GVRD8/ref=sr_1_59?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-59</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-21165-Minecraft-Building-Beekeeper/dp/B085WV8R86/ref=sr_1_60?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-60</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-Harry-Potter-75948-Confidential-Multi-Colour/dp/B07G3S3M9J/ref=sr_1_61?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570190&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-61</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-41444-Friends-Heartlake-Education/dp/B08G44DS1X/ref=sr_1_73?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570194&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-73</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/LEGO-Seasonal-Elf-Clubhouse-10275/dp/B08K94SH9G/ref=sr_1_97?crid=1SDTYPYXM70YV&amp;dchild=1&amp;keywords=lego&amp;qid=1634570197&amp;refinements=p_89%3Alego&amp;rnid=1632651031&amp;s=kids&amp;sprefix=my+li%2Ctoys%2C163&amp;sr=1-97</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t>4.3</t>
-  </si>
-  <si>
-    <t>5.0</t>
+    <t>4.5</t>
   </si>
   <si>
     <t>4.4</t>
   </si>
   <si>
+    <t>4.8</t>
+  </si>
+  <si>
     <t>4.9</t>
   </si>
   <si>
-    <t>4.8</t>
-  </si>
-  <si>
     <t>4.7</t>
   </si>
   <si>
     <t>4.6</t>
-  </si>
-  <si>
-    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -588,7 +804,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -616,16 +832,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C2">
-        <v>51.8</v>
+        <v>9.49</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>67</v>
+        <v>134</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -633,16 +849,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C3">
-        <v>25.97</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
+        <v>135</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -650,16 +866,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C4">
-        <v>9.99</v>
+        <v>239.74</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -667,16 +883,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>34.99</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -684,16 +900,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="C6">
-        <v>29.99</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" t="s">
-        <v>67</v>
+        <v>137</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -701,16 +917,16 @@
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C7">
         <v>36.99</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -718,16 +934,16 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C8">
-        <v>15</v>
+        <v>29.99</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -735,16 +951,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C9">
-        <v>99.98999999999999</v>
+        <v>27.99</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -752,16 +968,16 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C10">
-        <v>19.99</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -769,16 +985,16 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C11">
-        <v>30</v>
+        <v>19.99</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -786,16 +1002,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>59.8</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -803,16 +1019,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C13">
-        <v>13.99</v>
+        <v>8.99</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" t="s">
-        <v>67</v>
+        <v>138</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -820,16 +1036,16 @@
         <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="C14">
-        <v>8.99</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -837,16 +1053,16 @@
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C15">
-        <v>17.99</v>
+        <v>49.99</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" t="s">
-        <v>67</v>
+        <v>137</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -854,16 +1070,16 @@
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>19.99</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" t="s">
-        <v>67</v>
+        <v>138</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -871,16 +1087,16 @@
         <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C17">
-        <v>71.98999999999999</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -888,16 +1104,16 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C18">
-        <v>34.99</v>
+        <v>11.99</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -905,16 +1121,16 @@
         <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="C19">
-        <v>38.28</v>
+        <v>13.99</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -922,16 +1138,16 @@
         <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C20">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -939,16 +1155,16 @@
         <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C21">
-        <v>27.99</v>
+        <v>17.99</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" t="s">
-        <v>67</v>
+        <v>138</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -956,16 +1172,16 @@
         <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="C22">
-        <v>27.99</v>
+        <v>44.99</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -973,16 +1189,16 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="C23">
-        <v>17.99</v>
+        <v>71.98999999999999</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -990,16 +1206,16 @@
         <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="C24">
-        <v>35.99</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1007,16 +1223,16 @@
         <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="C25">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" t="s">
-        <v>67</v>
+        <v>138</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1024,16 +1240,16 @@
         <v>29</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="C26">
-        <v>11.99</v>
+        <v>34.99</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1041,16 +1257,16 @@
         <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="C27">
-        <v>14.99</v>
+        <v>17.99</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" t="s">
-        <v>67</v>
+        <v>136</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1058,16 +1274,696 @@
         <v>31</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28">
+        <v>29.99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29">
+        <v>34.99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30">
+        <v>49.99</v>
+      </c>
+      <c r="D30" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32">
+        <v>17.99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33">
+        <v>11.99</v>
+      </c>
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34">
+        <v>35.99</v>
+      </c>
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35">
+        <v>12.97</v>
+      </c>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38">
+        <v>14.99</v>
+      </c>
+      <c r="D38" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="D39" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40">
+        <v>31.99</v>
+      </c>
+      <c r="D40" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41">
+        <v>105.99</v>
+      </c>
+      <c r="D41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42">
+        <v>31.99</v>
+      </c>
+      <c r="D42" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43">
+        <v>59.99</v>
+      </c>
+      <c r="D43" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44">
+        <v>42.79</v>
+      </c>
+      <c r="D44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45">
+        <v>11.99</v>
+      </c>
+      <c r="D45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46">
+        <v>32.99</v>
+      </c>
+      <c r="D46" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47">
+        <v>9.49</v>
+      </c>
+      <c r="D47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48">
+        <v>27.99</v>
+      </c>
+      <c r="D48" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49">
+        <v>6.99</v>
+      </c>
+      <c r="D49" t="s">
+        <v>134</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C50" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52">
+        <v>8.93</v>
+      </c>
+      <c r="D52" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53">
+        <v>26.98</v>
+      </c>
+      <c r="D53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
+        <v>137</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55">
+        <v>17.99</v>
+      </c>
+      <c r="D55" t="s">
+        <v>138</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56">
+        <v>21.99</v>
+      </c>
+      <c r="D56" t="s">
+        <v>136</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>136</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58">
+        <v>16.99</v>
+      </c>
+      <c r="D58" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59">
+        <v>27.99</v>
+      </c>
+      <c r="D59" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60">
+        <v>109.99</v>
+      </c>
+      <c r="D60" t="s">
+        <v>137</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
         <v>58</v>
       </c>
-      <c r="C28">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B61" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" t="s">
+        <v>138</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62">
+        <v>31.98</v>
+      </c>
+      <c r="D62" t="s">
+        <v>136</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63">
+        <v>28</v>
+      </c>
+      <c r="D63" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64">
+        <v>17.99</v>
+      </c>
+      <c r="D64" t="s">
+        <v>138</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65">
+        <v>17.99</v>
+      </c>
+      <c r="D65" t="s">
+        <v>136</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66">
+        <v>66.95</v>
+      </c>
+      <c r="D66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
         <v>64</v>
       </c>
-      <c r="E28" t="s">
-        <v>67</v>
+      <c r="B67" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67">
+        <v>19.99</v>
+      </c>
+      <c r="D67" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68">
+        <v>84.98999999999999</v>
+      </c>
+      <c r="D68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E68">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1099,6 +1995,46 @@
     <hyperlink ref="B26" r:id="rId25"/>
     <hyperlink ref="B27" r:id="rId26"/>
     <hyperlink ref="B28" r:id="rId27"/>
+    <hyperlink ref="B29" r:id="rId28"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+    <hyperlink ref="B31" r:id="rId30"/>
+    <hyperlink ref="B32" r:id="rId31"/>
+    <hyperlink ref="B33" r:id="rId32"/>
+    <hyperlink ref="B34" r:id="rId33"/>
+    <hyperlink ref="B35" r:id="rId34"/>
+    <hyperlink ref="B36" r:id="rId35"/>
+    <hyperlink ref="B37" r:id="rId36"/>
+    <hyperlink ref="B38" r:id="rId37"/>
+    <hyperlink ref="B39" r:id="rId38"/>
+    <hyperlink ref="B40" r:id="rId39"/>
+    <hyperlink ref="B41" r:id="rId40"/>
+    <hyperlink ref="B42" r:id="rId41"/>
+    <hyperlink ref="B43" r:id="rId42"/>
+    <hyperlink ref="B44" r:id="rId43"/>
+    <hyperlink ref="B45" r:id="rId44"/>
+    <hyperlink ref="B46" r:id="rId45"/>
+    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="B48" r:id="rId47"/>
+    <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="B50" r:id="rId49"/>
+    <hyperlink ref="B51" r:id="rId50"/>
+    <hyperlink ref="B52" r:id="rId51"/>
+    <hyperlink ref="B53" r:id="rId52"/>
+    <hyperlink ref="B54" r:id="rId53"/>
+    <hyperlink ref="B55" r:id="rId54"/>
+    <hyperlink ref="B56" r:id="rId55"/>
+    <hyperlink ref="B57" r:id="rId56"/>
+    <hyperlink ref="B58" r:id="rId57"/>
+    <hyperlink ref="B59" r:id="rId58"/>
+    <hyperlink ref="B60" r:id="rId59"/>
+    <hyperlink ref="B61" r:id="rId60"/>
+    <hyperlink ref="B62" r:id="rId61"/>
+    <hyperlink ref="B63" r:id="rId62"/>
+    <hyperlink ref="B64" r:id="rId63"/>
+    <hyperlink ref="B65" r:id="rId64"/>
+    <hyperlink ref="B66" r:id="rId65"/>
+    <hyperlink ref="B67" r:id="rId66"/>
+    <hyperlink ref="B68" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>